<commit_message>
added Westgard Quality criteria
</commit_message>
<xml_diff>
--- a/example_data.xlsx
+++ b/example_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\augus\PycharmProjects\ARNlabIncertitudini\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9909B7E8-19BB-4425-BF13-3EFAE145C5F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243696CA-495C-47FC-B171-374A8E358537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C77CC0B5-667E-41EE-B57E-06188535CC80}"/>
   </bookViews>
@@ -485,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE51A86-D827-4C04-AAA0-C3B182E7E264}">
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1195,6 +1195,9 @@
       </c>
       <c r="M23" s="1"/>
     </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D24" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>